<commit_message>
Paso de Excel a Array en PHP
-Se logra colocar el Excel en un Array PHP (falta saber los métodos de
acceso al array.
</commit_message>
<xml_diff>
--- a/docs/ejerc1.xlsx
+++ b/docs/ejerc1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddinamarcat\Dropbox\Pega\CAS_LTDA\2016\Excel_Intermedio\Ejercicios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\erpcomin\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -843,11 +843,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="274275968"/>
-        <c:axId val="274276512"/>
+        <c:axId val="-1572155648"/>
+        <c:axId val="-1572146944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="274275968"/>
+        <c:axId val="-1572155648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -890,7 +890,7 @@
             <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274276512"/>
+        <c:crossAx val="-1572146944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -898,7 +898,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="274276512"/>
+        <c:axId val="-1572146944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -949,7 +949,7 @@
             <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274275968"/>
+        <c:crossAx val="-1572155648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -963,7 +963,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1060,7 +1059,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1268,11 +1266,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="274277056"/>
-        <c:axId val="274277600"/>
+        <c:axId val="-1572154016"/>
+        <c:axId val="-1572144224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="274277056"/>
+        <c:axId val="-1572154016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1315,7 +1313,7 @@
             <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274277600"/>
+        <c:crossAx val="-1572144224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1323,7 +1321,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="274277600"/>
+        <c:axId val="-1572144224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,7 +1372,7 @@
             <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274277056"/>
+        <c:crossAx val="-1572154016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1388,7 +1386,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1806,11 +1803,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="43609312"/>
-        <c:axId val="43609856"/>
+        <c:axId val="-1572157824"/>
+        <c:axId val="-1572146400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43609312"/>
+        <c:axId val="-1572157824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1853,7 +1850,7 @@
             <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43609856"/>
+        <c:crossAx val="-1572146400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1861,7 +1858,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43609856"/>
+        <c:axId val="-1572146400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1912,7 +1909,7 @@
             <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43609312"/>
+        <c:crossAx val="-1572157824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1926,7 +1923,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3882,7 +3878,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:D16" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0">
@@ -4024,7 +4020,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -4119,7 +4115,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:D8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">

</xml_diff>